<commit_message>
use . instead of ,
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidar\Documents\Rwd\ai_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9938784B-D6B0-4369-923D-A7120D533479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCFAA74-C1DB-4692-B737-2D27CE926DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20385" yWindow="3075" windowWidth="6315" windowHeight="10695" xr2:uid="{8021A6AD-FF9C-44B8-B823-FCF9A6CAB446}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8021A6AD-FF9C-44B8-B823-FCF9A6CAB446}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>date</t>
   </si>
@@ -75,18 +75,6 @@
   </si>
   <si>
     <t>FSLR</t>
-  </si>
-  <si>
-    <t>0,1</t>
-  </si>
-  <si>
-    <t>0,25</t>
-  </si>
-  <si>
-    <t>0,2</t>
-  </si>
-  <si>
-    <t>0,5</t>
   </si>
 </sst>
 </file>
@@ -462,7 +450,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,8 +476,8 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
+      <c r="C2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -499,8 +487,8 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
+      <c r="C3">
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -510,8 +498,8 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
+      <c r="C4">
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -521,8 +509,8 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
+      <c r="C5">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -532,8 +520,8 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
+      <c r="C6">
+        <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -543,8 +531,8 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
+      <c r="C7">
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -554,8 +542,8 @@
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
-        <v>13</v>
+      <c r="C8">
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -565,8 +553,8 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>13</v>
+      <c r="C9">
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,8 +564,8 @@
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
+      <c r="C10">
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,8 +575,8 @@
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
-        <v>13</v>
+      <c r="C11">
+        <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,8 +586,8 @@
       <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
-        <v>14</v>
+      <c r="C12">
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -609,8 +597,8 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
+      <c r="C13">
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,8 +608,8 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
+      <c r="C14">
+        <v>0.2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,8 +619,8 @@
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
-        <v>13</v>
+      <c r="C15">
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,8 +630,8 @@
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" t="s">
-        <v>13</v>
+      <c r="C16">
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,8 +641,8 @@
       <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
-        <v>13</v>
+      <c r="C17">
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,8 +652,8 @@
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" t="s">
-        <v>16</v>
+      <c r="C18">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix calculations regarding rebalancing and add claude.md
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidar\Documents\Rwd\ai_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D5E229-C1F5-42F9-9F51-49529F237C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1314435C-3BF1-4E8E-AA6B-4FA52C42967F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8021A6AD-FF9C-44B8-B823-FCF9A6CAB446}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8021A6AD-FF9C-44B8-B823-FCF9A6CAB446}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76405F02-88FB-4385-9399-EAE5923F1017}">
   <dimension ref="A1:D878"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update medium risk portfolio
</commit_message>
<xml_diff>
--- a/portfolio.xlsx
+++ b/portfolio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vidar\Documents\Rwd\ai_portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307931FC-0C3C-49C7-8FA7-48EF6504E386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E7CD8-B43F-4B28-94BD-8B4DADADE47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8021A6AD-FF9C-44B8-B823-FCF9A6CAB446}"/>
   </bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="A1:D871"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +989,7 @@
         <v>26</v>
       </c>
       <c r="B34" s="1">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="C34" t="s">
         <v>16</v>
@@ -1003,7 +1003,7 @@
         <v>26</v>
       </c>
       <c r="B35" s="1">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="C35" t="s">
         <v>27</v>
@@ -1017,7 +1017,7 @@
         <v>26</v>
       </c>
       <c r="B36" s="1">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="C36" t="s">
         <v>28</v>
@@ -1031,7 +1031,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="1">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="C37" t="s">
         <v>29</v>
@@ -1045,7 +1045,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="1">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="C38" t="s">
         <v>30</v>
@@ -1059,7 +1059,7 @@
         <v>26</v>
       </c>
       <c r="B39" s="1">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="C39" t="s">
         <v>31</v>
@@ -1073,7 +1073,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="1">
-        <v>45929</v>
+        <v>45935</v>
       </c>
       <c r="C40" t="s">
         <v>32</v>

</xml_diff>